<commit_message>
Added Streamlit chat app
</commit_message>
<xml_diff>
--- a/WHO_FAQ.xlsx
+++ b/WHO_FAQ.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="125">
   <si>
     <t>Context</t>
   </si>
@@ -43,10 +43,7 @@
     <t>The most common symptoms of COVID-19 are fever, tiredness, and dry cough. Some patients may have aches and pains, nasal congestion, runny nose, sore throat or diarrhea. These symptoms are usually mild and begin gradually.</t>
   </si>
   <si>
-    <t>Some people become infected but don’t develop any symptoms and don't feel unwell. Most people (about 80%) recover from the disease without needing special treatment.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Around 1 out of every 6 people who gets COVID-19 becomes seriously ill and develops difficulty breathing. </t>
+    <t xml:space="preserve">The most common symptoms of COVID-19 are fever, tiredness, and dry cough. Around 1 out of every 6 people who gets COVID-19 becomes seriously ill and develops difficulty breathing. </t>
   </si>
   <si>
     <t>Older people, and those with underlying medical problems like high blood pressure, heart problems or diabetes, are more likely to develop serious illness. People with fever, cough and difficulty breathing should seek medical attention.</t>
@@ -85,13 +82,13 @@
     <t>What can I do to protect myself and prevent the spread of disease?</t>
   </si>
   <si>
-    <t>Regularly and thoroughly clean your hands with an alcohol-based hand rub or wash them with soap and water.</t>
-  </si>
-  <si>
-    <t>Maintain at least 1 metre (3 feet) distance between yourself and anyone who is coughing or sneezing.</t>
-  </si>
-  <si>
-    <t>Avoid touching eyes, nose and mouth.</t>
+    <t>Regularly and thoroughly clean your hands with an alcohol-based hand rub or wash them with soap and water. Maintain at least 1 metre (3 feet) distance between yourself and anyone who is coughing or sneezing. Avoid touching eyes, nose and mouth.</t>
+  </si>
+  <si>
+    <t>How can I protect myself from this virus ?</t>
+  </si>
+  <si>
+    <t>Maintain at least 1 metre (3 feet) distance between yourself and anyone who is coughing or sneezing. Avoid touching eyes, nose and mouth.</t>
   </si>
   <si>
     <t>Make sure you, and the people around you, follow good respiratory hygiene. This means covering your mouth and nose with your bent elbow or tissue when you cough or sneeze. Then dispose of the used tissue immediately.</t>
@@ -100,10 +97,7 @@
     <t>Stay home if you feel unwell. If you have a fever, cough and difficulty breathing, seek medical attention and call in advance. Follow the directions of your local health authority.</t>
   </si>
   <si>
-    <t>If possible, avoid traveling to places  – especially if you are an older person or have diabetes, heart or lung disease.</t>
-  </si>
-  <si>
-    <t>Keep up to date on the latest COVID-19 hotspots (cities or local areas where COVID-19 is spreading widely).</t>
+    <t>If possible, avoid traveling to places  – especially if you are an older person or have diabetes, heart or lung disease. Keep up to date on the latest COVID-19 hotspots (cities or local areas where COVID-19 is spreading widely).</t>
   </si>
   <si>
     <t>What can I do to protect myself andProtection measures for persons who are in or have recently visited (past 14 days) areas where COVID-19 is spreading prevent the spread of disease?</t>
@@ -136,9 +130,6 @@
     <t>Illness due to COVID-19 infection is generally mild, especially for children and young adults. However, it can cause serious illness: about 1 in every 5 people who catch it need hospital care.</t>
   </si>
   <si>
-    <t>We can channel our concerns into actions to protect ourselves, our loved ones and our communities.</t>
-  </si>
-  <si>
     <t>Who is at risk of developing severe illness?</t>
   </si>
   <si>
@@ -157,9 +148,6 @@
     <t>Are there any medicines or therapies that can prevent or cure COVID-19?</t>
   </si>
   <si>
-    <t xml:space="preserve">While some western, traditional or home remedies may provide comfort and alleviate symptoms of COVID-19, there is no evidence that current medicine can prevent or cure the disease. </t>
-  </si>
-  <si>
     <t>WHO does not recommend self-medication with any medicines, including antibiotics, as a prevention or cure for COVID-19.</t>
   </si>
   <si>
@@ -178,7 +166,7 @@
     <t>Where to get  should I get the vaccines?</t>
   </si>
   <si>
-    <t>Vaccines are available from Government and Private Health Facilities as notified, known as COVID Vaccination Centres (CVCs). Visit https://www.mohfw.gov.in/ and register yourself for the vaccine shot.</t>
+    <t>Vaccines are available from Government and Private Health Facilities as notified, known as COVID Vaccination Centres (CVCs). Visit https://www.cowin.gov.in/ and register yourself for the vaccine shot.</t>
   </si>
   <si>
     <t>Is COVID-19 the same as SARS?</t>
@@ -250,13 +238,10 @@
     <t>How long does the virus survive on surfaces?</t>
   </si>
   <si>
-    <t>It is not certain how long the virus that causes COVID-19 survives on surfaces, but it seems to behave like other coronaviruses.</t>
+    <t>It is not certain how long the virus that causes COVID-19 survives on surfaces, but it seems to behave like other coronaviruses. Studies suggest that coronaviruses (including preliminary information on the COVID-19 virus) may persist on surfaces for a few hours or up to several days. This may vary under different conditions (e.g. type of surface, temperature or humidity of the environment).</t>
   </si>
   <si>
     <t>Studies suggest that coronaviruses (including preliminary information on the COVID-19 virus) may persist on surfaces for a few hours or up to several days. This may vary under different conditions (e.g. type of surface, temperature or humidity of the environment).</t>
-  </si>
-  <si>
-    <t>If you think a surface may be infected, clean it with simple disinfectant to kill the virus and protect yourself and others.</t>
   </si>
   <si>
     <t>Is it safe to receive a package from any area where COVID-19 has been reported?</t>
@@ -411,7 +396,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -435,6 +420,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri (Hoofdtekst)"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -482,13 +473,13 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -799,14 +790,14 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C111"/>
+  <dimension ref="A1:C105"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="7" width="70.7192857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="178.29071428571427" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="244.29071428571427" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
@@ -875,16 +866,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>13</v>
@@ -892,26 +883,26 @@
       <c r="C9" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="1" t="s">
-        <v>12</v>
+      <c r="A10" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C11" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>18</v>
@@ -920,91 +911,91 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C13" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C14" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C15" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="C16" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="C17" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C18" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="C19" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="1" t="s">
-        <v>22</v>
+      <c r="A20" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C20" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
-      <c r="A21" s="1" t="s">
-        <v>22</v>
+      <c r="A21" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C21" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="1" t="s">
-        <v>30</v>
+      <c r="A22" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C22" s="1"/>
     </row>
@@ -1013,566 +1004,542 @@
         <v>32</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C23" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
-      <c r="A24" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>35</v>
+      <c r="A24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="C24" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
-      <c r="A25" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>36</v>
+      <c r="A25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="C25" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
-      <c r="A26" s="2" t="s">
-        <v>34</v>
+      <c r="A26" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C26" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="C27" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
       <c r="A28" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C28" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
-      <c r="A29" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C29" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
+      <c r="A29" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="5"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
       <c r="A30" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C30" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
       <c r="A31" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C31" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
       <c r="A32" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C32" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25">
       <c r="A33" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C33" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
-      <c r="A34" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C34" s="5"/>
+      <c r="A34" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25">
       <c r="A35" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C35" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25">
       <c r="A36" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C36" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25">
       <c r="A37" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C37" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25">
       <c r="A38" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C38" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25">
       <c r="A39" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C39" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="17.25">
       <c r="A40" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C40" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="17.25">
       <c r="A41" s="1" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C41" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="17.25">
       <c r="A42" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C42" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="17.25">
       <c r="A43" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C43" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="17.25">
       <c r="A44" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C44" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="17.25">
       <c r="A45" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C45" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="17.25">
       <c r="A46" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C46" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="17.25">
       <c r="A47" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C47" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="17.25">
       <c r="A48" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C48" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="17.25">
       <c r="A49" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C49" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="17.25">
       <c r="A50" s="1" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C50" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="17.25">
       <c r="A51" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C51" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="17.25">
       <c r="A52" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C52" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="17.25">
       <c r="A53" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C53" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="17.25">
       <c r="A54" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C54" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="17.25">
       <c r="A55" s="1" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C55" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="17.25">
       <c r="A56" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C56" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="17.25">
       <c r="A57" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C57" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="17.25">
       <c r="A58" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>85</v>
+        <v>88</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="C58" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="17.25">
       <c r="A59" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="C59" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="17.25">
       <c r="A60" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="C60" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="17.25">
       <c r="A61" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C61" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="17.25">
       <c r="A62" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C62" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="17.25">
       <c r="A63" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>92</v>
+        <v>96</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="C63" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="17.25">
       <c r="A64" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>99</v>
       </c>
       <c r="C64" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="17.25">
       <c r="A65" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="C65" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="17.25">
       <c r="A66" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>97</v>
+        <v>102</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>103</v>
       </c>
       <c r="C66" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="17.25">
       <c r="A67" s="1" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="C67" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="17.25">
       <c r="A68" s="1" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="C68" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="17.25">
       <c r="A69" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>102</v>
+        <v>108</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>109</v>
       </c>
       <c r="C69" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="17.25">
       <c r="A70" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>110</v>
       </c>
       <c r="C70" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="17.25">
       <c r="A71" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>106</v>
+        <v>111</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>112</v>
       </c>
       <c r="C71" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="17.25">
       <c r="A72" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>108</v>
+        <v>111</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>113</v>
       </c>
       <c r="C72" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="17.25">
       <c r="A73" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>114</v>
       </c>
       <c r="C73" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="17.25">
       <c r="A74" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>116</v>
       </c>
       <c r="C74" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="17.25">
       <c r="A75" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B75" s="6" t="s">
-        <v>114</v>
+        <v>117</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="C75" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="17.25">
       <c r="A76" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C76" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="17.25">
       <c r="A77" s="1" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C77" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="17.25">
       <c r="A78" s="1" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C78" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="17.25">
       <c r="A79" s="1" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="C79" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="17.25">
-      <c r="A80" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B80" s="6" t="s">
-        <v>121</v>
-      </c>
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
       <c r="C80" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="17.25">
-      <c r="A81" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>123</v>
-      </c>
+      <c r="A81" s="6"/>
+      <c r="B81" s="1"/>
       <c r="C81" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="17.25">
-      <c r="A82" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B82" s="6" t="s">
-        <v>124</v>
-      </c>
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
       <c r="C82" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="17.25">
-      <c r="A83" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B83" s="6" t="s">
-        <v>126</v>
-      </c>
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
       <c r="C83" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="17.25">
-      <c r="A84" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B84" s="6" t="s">
-        <v>127</v>
-      </c>
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
       <c r="C84" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="17.25">
-      <c r="A85" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B85" s="6" t="s">
-        <v>129</v>
-      </c>
+      <c r="A85" s="1"/>
+      <c r="B85" s="1"/>
       <c r="C85" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="17.25">
@@ -1581,7 +1548,7 @@
       <c r="C86" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="17.25">
-      <c r="A87" s="6"/>
+      <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
     </row>
@@ -1591,37 +1558,37 @@
       <c r="C88" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="17.25">
-      <c r="A89" s="1"/>
+      <c r="A89" s="4"/>
       <c r="B89" s="1"/>
-      <c r="C89" s="1"/>
+      <c r="C89" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="17.25">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
-      <c r="C90" s="1"/>
+      <c r="C90" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="17.25">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
-      <c r="C91" s="1"/>
+      <c r="C91" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="17.25">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
-      <c r="C92" s="1"/>
+      <c r="C92" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="17.25">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
-      <c r="C93" s="1"/>
+      <c r="C93" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="17.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
-      <c r="C94" s="1"/>
+      <c r="C94" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="17.25">
-      <c r="A95" s="4"/>
+      <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="5"/>
     </row>
@@ -1675,36 +1642,6 @@
       <c r="B105" s="1"/>
       <c r="C105" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="17.25">
-      <c r="A106" s="1"/>
-      <c r="B106" s="1"/>
-      <c r="C106" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="17.25">
-      <c r="A107" s="1"/>
-      <c r="B107" s="1"/>
-      <c r="C107" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="17.25">
-      <c r="A108" s="1"/>
-      <c r="B108" s="1"/>
-      <c r="C108" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="17.25">
-      <c r="A109" s="1"/>
-      <c r="B109" s="1"/>
-      <c r="C109" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="17.25">
-      <c r="A110" s="1"/>
-      <c r="B110" s="1"/>
-      <c r="C110" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="17.25">
-      <c r="A111" s="1"/>
-      <c r="B111" s="1"/>
-      <c r="C111" s="5"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>